<commit_message>
he vuelto a subir el programa completo
</commit_message>
<xml_diff>
--- a/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_FITOS_P2_2025.xlsx
+++ b/LISTADO_PEDIDO_COMPRAS/data/input/CLASIFICACION_ABC+D_FITOS_P2_2025.xlsx
@@ -5984,12 +5984,12 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>3302080002</t>
+          <t>3302200022</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>ABONO LIQUIDO GERANIOS 1300ML</t>
+          <t>COMPO TURBO RAICES 50GR</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr"/>
@@ -6008,71 +6008,71 @@
         <v>90</v>
       </c>
       <c r="H65" s="4" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I65" s="4" t="n">
-        <v>107.86</v>
+        <v>99.34999999999999</v>
       </c>
       <c r="J65" s="4" t="n">
-        <v>40.14</v>
+        <v>33.11</v>
       </c>
       <c r="K65" s="4" t="n">
-        <v>0</v>
+        <v>83.33</v>
       </c>
       <c r="L65" s="4" t="n">
         <v>0</v>
       </c>
       <c r="M65" s="5" t="n">
-        <v>6.8</v>
+        <v>12.2</v>
       </c>
       <c r="N65" s="5" t="n">
-        <v>20.5</v>
+        <v>36.7</v>
       </c>
       <c r="O65" s="4" t="n">
-        <v>-14</v>
+        <v>5</v>
       </c>
       <c r="P65" s="4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q65" s="4" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="R65" s="4" t="n">
-        <v>0</v>
+        <v>86.67</v>
       </c>
       <c r="S65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T65" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>10</v>
+      </c>
+      <c r="T65" s="7" t="inlineStr">
+        <is>
+          <t>Medio</t>
         </is>
       </c>
       <c r="U65" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -14 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>REPOSICIÓN SELECTIVA: Aumentar compras 15% para evitar ruptura de stock. Aplicar descuento 5% para consolidar demanda.</t>
         </is>
       </c>
       <c r="V65" s="4" t="inlineStr">
         <is>
-          <t>Sin stock</t>
+          <t>Compra 14/03/2025</t>
         </is>
       </c>
       <c r="W65" s="4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>3302200022</t>
+          <t>3302080002</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>COMPO TURBO RAICES 50GR</t>
+          <t>ABONO LIQUIDO GERANIOS 1300ML</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr"/>
@@ -6091,59 +6091,59 @@
         <v>90</v>
       </c>
       <c r="H66" s="4" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I66" s="4" t="n">
-        <v>99.34999999999999</v>
+        <v>107.86</v>
       </c>
       <c r="J66" s="4" t="n">
-        <v>33.11</v>
+        <v>40.14</v>
       </c>
       <c r="K66" s="4" t="n">
-        <v>83.33</v>
+        <v>0</v>
       </c>
       <c r="L66" s="4" t="n">
         <v>0</v>
       </c>
       <c r="M66" s="5" t="n">
-        <v>12.2</v>
+        <v>6.8</v>
       </c>
       <c r="N66" s="5" t="n">
-        <v>36.7</v>
+        <v>20.5</v>
       </c>
       <c r="O66" s="4" t="n">
-        <v>5</v>
+        <v>-14</v>
       </c>
       <c r="P66" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q66" s="4" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="R66" s="4" t="n">
-        <v>86.67</v>
+        <v>0</v>
       </c>
       <c r="S66" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="T66" s="7" t="inlineStr">
-        <is>
-          <t>Medio</t>
+        <v>0</v>
+      </c>
+      <c r="T66" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U66" s="3" t="inlineStr">
         <is>
-          <t>REPOSICIÓN SELECTIVA: Aumentar compras 15% para evitar ruptura de stock. Aplicar descuento 5% para consolidar demanda.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -14 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V66" s="4" t="inlineStr">
         <is>
-          <t>Compra 14/03/2025</t>
+          <t>Sin stock</t>
         </is>
       </c>
       <c r="W66" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
     </row>
@@ -12618,37 +12618,37 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>3302120001</t>
+          <t>3901140001</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>ABONO LIQUIDO FRESALES Y FRUTOS ROJOS 500ML</t>
+          <t>ECO-STOP CUCANOR 750ML</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr"/>
       <c r="D47" s="3" t="inlineStr"/>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>ANTI-PLAGAS</t>
         </is>
       </c>
       <c r="G47" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I47" s="4" t="n">
-        <v>42.45</v>
+        <v>43.8</v>
       </c>
       <c r="J47" s="4" t="n">
-        <v>16.98</v>
+        <v>18.1</v>
       </c>
       <c r="K47" s="4" t="n">
         <v>0</v>
@@ -12657,16 +12657,16 @@
         <v>0</v>
       </c>
       <c r="M47" s="5" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="N47" s="5" t="n">
-        <v>7.3</v>
+        <v>5.9</v>
       </c>
       <c r="O47" s="4" t="n">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="P47" s="4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q47" s="4" t="n">
         <v>0</v>
@@ -12684,7 +12684,7 @@
       </c>
       <c r="U47" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -5 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V47" s="4" t="inlineStr">
@@ -12701,37 +12701,37 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>3901140001</t>
+          <t>3302120001</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>ECO-STOP CUCANOR 750ML</t>
+          <t>ABONO LIQUIDO FRESALES Y FRUTOS ROJOS 500ML</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr"/>
       <c r="D48" s="3" t="inlineStr"/>
       <c r="E48" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F48" s="4" t="inlineStr">
         <is>
-          <t>ANTI-PLAGAS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G48" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H48" s="4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I48" s="4" t="n">
-        <v>43.8</v>
+        <v>42.45</v>
       </c>
       <c r="J48" s="4" t="n">
-        <v>18.1</v>
+        <v>16.98</v>
       </c>
       <c r="K48" s="4" t="n">
         <v>0</v>
@@ -12740,16 +12740,16 @@
         <v>0</v>
       </c>
       <c r="M48" s="5" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="N48" s="5" t="n">
-        <v>5.9</v>
+        <v>7.3</v>
       </c>
       <c r="O48" s="4" t="n">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="P48" s="4" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q48" s="4" t="n">
         <v>0</v>
@@ -12767,7 +12767,7 @@
       </c>
       <c r="U48" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 20% próxima temporada. Stock actual: -5 unidades. Stock objetivo: 1 unidades. Maximizar disponibilidad.</t>
         </is>
       </c>
       <c r="V48" s="4" t="inlineStr">
@@ -16034,37 +16034,37 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>3601050007</t>
+          <t>3302200025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>VITHAL LIMPIA MELAZAS 750ML JABON NEGRO</t>
+          <t>VARITAS PLANTAS VERDES 30 ST</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
       <c r="D16" s="3" t="inlineStr"/>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIO NATURAL</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G16" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>25.5</v>
+        <v>23</v>
       </c>
       <c r="J16" s="4" t="n">
-        <v>10.27</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="K16" s="4" t="n">
         <v>0</v>
@@ -16073,16 +16073,16 @@
         <v>0</v>
       </c>
       <c r="M16" s="5" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>4.4</v>
+        <v>5.9</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="Q16" s="4" t="n">
         <v>0</v>
@@ -16100,7 +16100,7 @@
       </c>
       <c r="U16" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -3 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
         </is>
       </c>
       <c r="V16" s="4" t="inlineStr">
@@ -16117,37 +16117,37 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>3302200025</t>
+          <t>3601050007</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>VARITAS PLANTAS VERDES 30 ST</t>
+          <t>VITHAL LIMPIA MELAZAS 750ML JABON NEGRO</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr"/>
       <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIO NATURAL</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>23</v>
+        <v>25.5</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>8.210000000000001</v>
+        <v>10.27</v>
       </c>
       <c r="K17" s="4" t="n">
         <v>0</v>
@@ -16156,16 +16156,16 @@
         <v>0</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="N17" s="5" t="n">
-        <v>5.9</v>
+        <v>4.4</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="4" t="n">
         <v>0</v>
@@ -16183,7 +16183,7 @@
       </c>
       <c r="U17" s="3" t="inlineStr">
         <is>
-          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -4 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
+          <t>AUMENTAR STOCK: Producto de alto interés. Incrementar compras 30% próxima temporada. Stock actual: -3 unidades. Stock objetivo: 1 unidades. Alta rotación confirmada.</t>
         </is>
       </c>
       <c r="V17" s="4" t="inlineStr">
@@ -16805,12 +16805,12 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>3502010005</t>
+          <t>3501100025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO HU AZUFRE 450GR</t>
+          <t>MASTI-CORT CICATRIZANTE 250GR</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr"/>
@@ -16832,10 +16832,10 @@
         <v>2</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>20.98</v>
+        <v>19.93</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>8.300000000000001</v>
+        <v>7.43</v>
       </c>
       <c r="K25" s="4" t="n">
         <v>8.33</v>
@@ -16853,47 +16853,47 @@
         <v>22</v>
       </c>
       <c r="P25" s="4" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q25" s="4" t="n">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="R25" s="4" t="n">
-        <v>102.22</v>
+        <v>63.33</v>
       </c>
       <c r="S25" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="T25" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>0</v>
+      </c>
+      <c r="T25" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U25" s="3" t="inlineStr">
         <is>
-          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
+          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 1012 días.</t>
         </is>
       </c>
       <c r="V25" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 04/04/2025</t>
         </is>
       </c>
       <c r="W25" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>3501100025</t>
+          <t>3502010005</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>MASTI-CORT CICATRIZANTE 250GR</t>
+          <t>COMPO BIO HU AZUFRE 450GR</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr"/>
@@ -16915,10 +16915,10 @@
         <v>2</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>19.93</v>
+        <v>20.98</v>
       </c>
       <c r="J26" s="4" t="n">
-        <v>7.43</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="K26" s="4" t="n">
         <v>8.33</v>
@@ -16936,35 +16936,35 @@
         <v>22</v>
       </c>
       <c r="P26" s="4" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="4" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="R26" s="4" t="n">
-        <v>63.33</v>
+        <v>102.22</v>
       </c>
       <c r="S26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>20</v>
+      </c>
+      <c r="T26" s="8" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
       <c r="U26" s="3" t="inlineStr">
         <is>
-          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 1012 días.</t>
+          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
         </is>
       </c>
       <c r="V26" s="4" t="inlineStr">
         <is>
-          <t>Compra 04/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W26" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
     </row>
@@ -18556,186 +18556,186 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>3302010002</t>
+          <t>3502010011</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>ABONO CONIFERAS Y SETOS 750GR</t>
-        </is>
-      </c>
-      <c r="C46" s="3" t="inlineStr"/>
-      <c r="D46" s="3" t="inlineStr"/>
+          <t>COMPO FUNGICIDA PHITOFTORA</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>45GR</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>UNICO</t>
+        </is>
+      </c>
       <c r="E46" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F46" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G46" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H46" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" s="4" t="n">
+        <v>11.38</v>
+      </c>
+      <c r="J46" s="4" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="K46" s="4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L46" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I46" s="4" t="n">
-        <v>10.95</v>
-      </c>
-      <c r="J46" s="4" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="K46" s="4" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="L46" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" s="5" t="n">
-        <v>0.5</v>
-      </c>
       <c r="N46" s="5" t="n">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="O46" s="4" t="n">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="P46" s="4" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="Q46" s="4" t="n">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="R46" s="4" t="n">
-        <v>35.56</v>
+        <v>102.22</v>
       </c>
       <c r="S46" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T46" s="6" t="inlineStr">
-        <is>
-          <t>Bajo</t>
+        <v>20</v>
+      </c>
+      <c r="T46" s="8" t="inlineStr">
+        <is>
+          <t>Alto</t>
         </is>
       </c>
       <c r="U46" s="3" t="inlineStr">
         <is>
-          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 644 días.</t>
+          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
         </is>
       </c>
       <c r="V46" s="4" t="inlineStr">
         <is>
-          <t>Compra 29/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W46" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>3502010011</t>
+          <t>3302010002</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>COMPO FUNGICIDA PHITOFTORA</t>
-        </is>
-      </c>
-      <c r="C47" s="3" t="inlineStr">
-        <is>
-          <t>45GR</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="inlineStr">
-        <is>
-          <t>UNICO</t>
-        </is>
-      </c>
+          <t>ABONO CONIFERAS Y SETOS 750GR</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr"/>
+      <c r="D47" s="3" t="inlineStr"/>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G47" s="4" t="n">
         <v>90</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" s="4" t="n">
-        <v>11.38</v>
+        <v>10.95</v>
       </c>
       <c r="J47" s="4" t="n">
-        <v>4.42</v>
+        <v>4.07</v>
       </c>
       <c r="K47" s="4" t="n">
-        <v>2.5</v>
+        <v>12.5</v>
       </c>
       <c r="L47" s="4" t="n">
         <v>0</v>
       </c>
       <c r="M47" s="5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N47" s="5" t="n">
-        <v>2.9</v>
+        <v>1.5</v>
       </c>
       <c r="O47" s="4" t="n">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="P47" s="4" t="n">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="Q47" s="4" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="R47" s="4" t="n">
-        <v>102.22</v>
+        <v>35.56</v>
       </c>
       <c r="S47" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="T47" s="8" t="inlineStr">
-        <is>
-          <t>Alto</t>
+        <v>0</v>
+      </c>
+      <c r="T47" s="6" t="inlineStr">
+        <is>
+          <t>Bajo</t>
         </is>
       </c>
       <c r="U47" s="3" t="inlineStr">
         <is>
-          <t>REDUCCIÓN AGRESIVA: Aplicar descuento 20% inmediato. Reducir compras 70% próxima temporada. Stock objetivo: 1 unidades. Riesgo alto de merma.</t>
+          <t>MANTENER SIN DESCUENTO: Stock fresco de calidad. Reducir compras 25% próxima temporada. Stock actual suficiente para 644 días.</t>
         </is>
       </c>
       <c r="V47" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 29/04/2025</t>
         </is>
       </c>
       <c r="W47" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>3502010007</t>
+          <t>3502010014</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>BIOFLOWER FUNGIBAC COLA CABALLO 50ML</t>
+          <t>REVUS ANTIMILDIU 20ML</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr"/>
@@ -18778,7 +18778,7 @@
         <v>-1</v>
       </c>
       <c r="P48" s="4" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="Q48" s="4" t="n">
         <v>0</v>
@@ -18813,12 +18813,12 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>3502010014</t>
+          <t>3502010007</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>REVUS ANTIMILDIU 20ML</t>
+          <t>BIOFLOWER FUNGIBAC COLA CABALLO 50ML</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr"/>
@@ -18861,7 +18861,7 @@
         <v>-1</v>
       </c>
       <c r="P49" s="4" t="n">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="Q49" s="4" t="n">
         <v>0</v>
@@ -20470,12 +20470,12 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>3501010004</t>
+          <t>3501100016</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>TRIPLE ACCION 1000ML AFIDOR</t>
+          <t>YNJECT CONECTOR PALMERA (NO VENTA)</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr"/>
@@ -20506,7 +20506,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>0</v>
@@ -20515,19 +20515,19 @@
         <v>0</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="P2" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q2" s="4" t="n">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="R2" s="4" t="n">
-        <v>36.67</v>
+        <v>102.22</v>
       </c>
       <c r="S2" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T2" s="9" t="inlineStr">
         <is>
@@ -20536,12 +20536,12 @@
       </c>
       <c r="U2" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 23.52€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V2" s="4" t="inlineStr">
         <is>
-          <t>Compra 28/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W2" s="4" t="inlineStr">
@@ -20553,12 +20553,12 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>3301040006</t>
+          <t>3302170002</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO FERTILIZANTE AQUA DEPOT 1L</t>
+          <t>ABONO UNIVERSAL 1,5KG</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr"/>
@@ -20589,7 +20589,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="4" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>0</v>
@@ -20598,19 +20598,19 @@
         <v>0</v>
       </c>
       <c r="O3" s="4" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="P3" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="R3" s="4" t="n">
-        <v>86.67</v>
+        <v>102.22</v>
       </c>
       <c r="S3" s="5" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="T3" s="9" t="inlineStr">
         <is>
@@ -20619,12 +20619,12 @@
       </c>
       <c r="U3" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 10% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 50.4€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V3" s="4" t="inlineStr">
         <is>
-          <t>Compra 14/03/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W3" s="4" t="inlineStr">
@@ -20636,24 +20636,24 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>3701010006</t>
+          <t>3301040006</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>HERBICIDA DUO (FLUROXI + QUIZALOF)</t>
+          <t>COMPO BIO FERTILIZANTE AQUA DEPOT 1L</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr"/>
       <c r="D4" s="3" t="inlineStr"/>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>HERBICIDAS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
@@ -20672,7 +20672,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>0</v>
@@ -20681,19 +20681,19 @@
         <v>0</v>
       </c>
       <c r="O4" s="4" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P4" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q4" s="4" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="R4" s="4" t="n">
-        <v>102.22</v>
+        <v>86.67</v>
       </c>
       <c r="S4" s="5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="T4" s="9" t="inlineStr">
         <is>
@@ -20702,12 +20702,12 @@
       </c>
       <c r="U4" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 71.75€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 10% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V4" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 14/03/2025</t>
         </is>
       </c>
       <c r="W4" s="4" t="inlineStr">
@@ -20719,24 +20719,24 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>3302210005</t>
+          <t>3501100022</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>CANABIUM VITACANN BIOESTIMULADOR 250ML</t>
+          <t>YNJECT GO PALMERAS (NO VENTA)</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="3" t="inlineStr"/>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G5" s="4" t="n">
@@ -20755,7 +20755,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>0</v>
@@ -20764,19 +20764,19 @@
         <v>0</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="P5" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="R5" s="4" t="n">
-        <v>36.67</v>
+        <v>102.22</v>
       </c>
       <c r="S5" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="9" t="inlineStr">
         <is>
@@ -20785,12 +20785,12 @@
       </c>
       <c r="U5" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 211.68€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V5" s="4" t="inlineStr">
         <is>
-          <t>Compra 28/04/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W5" s="4" t="inlineStr">
@@ -20802,12 +20802,12 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>3501100016</t>
+          <t>3501100021</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>YNJECT CONECTOR PALMERA (NO VENTA)</t>
+          <t>YNJECT GO PINO (NO VENTA)</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr"/>
@@ -20838,7 +20838,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>0</v>
@@ -20847,7 +20847,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="P6" s="4" t="n">
         <v>92</v>
@@ -20868,7 +20868,7 @@
       </c>
       <c r="U6" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 23.52€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 47.04€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V6" s="4" t="inlineStr">
@@ -20885,24 +20885,24 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>3302170002</t>
+          <t>3901160000</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>ABONO UNIVERSAL 1,5KG</t>
+          <t>FIN DESINFECTANTE SUPERFICIES 1L LU</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" s="3" t="inlineStr"/>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>ANTI-PLAGAS</t>
         </is>
       </c>
       <c r="G7" s="4" t="n">
@@ -20921,7 +20921,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="M7" s="5" t="n">
         <v>0</v>
@@ -20930,19 +20930,19 @@
         <v>0</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P7" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q7" s="4" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="R7" s="4" t="n">
-        <v>102.22</v>
+        <v>17.78</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T7" s="9" t="inlineStr">
         <is>
@@ -20951,12 +20951,12 @@
       </c>
       <c r="U7" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 50.4€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V7" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 15/05/2025</t>
         </is>
       </c>
       <c r="W7" s="4" t="inlineStr">
@@ -20968,12 +20968,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>3301080002</t>
+          <t>3302210008</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>COMPO REVIT ORQUIDEA MONODOSIS 5X30ML</t>
+          <t>FERTILIZANTE ORQUIDEAS 250ML</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
@@ -21051,12 +21051,12 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>3302210008</t>
+          <t>3302210016</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>FERTILIZANTE ORQUIDEAS 250ML</t>
+          <t>VIGORIZANTE FOLIAR CACTUS Y CRASAS 250ML</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr"/>
@@ -21087,7 +21087,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M9" s="5" t="n">
         <v>0</v>
@@ -21096,16 +21096,16 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P9" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="R9" s="4" t="n">
-        <v>4.44</v>
+        <v>63.33</v>
       </c>
       <c r="S9" s="5" t="n">
         <v>0</v>
@@ -21122,7 +21122,7 @@
       </c>
       <c r="V9" s="4" t="inlineStr">
         <is>
-          <t>Compra 27/05/2025</t>
+          <t>Compra 04/04/2025</t>
         </is>
       </c>
       <c r="W9" s="4" t="inlineStr">
@@ -21134,12 +21134,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>3501100015</t>
+          <t>3502020004</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>YNJECT CONECTOR PINO (NO VENTA)</t>
+          <t>COMPO BIO FUNGICIDA STOP 750ML</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr"/>
@@ -21170,7 +21170,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="M10" s="5" t="n">
         <v>0</v>
@@ -21179,19 +21179,19 @@
         <v>0</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="P10" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>92</v>
+        <v>4</v>
       </c>
       <c r="R10" s="4" t="n">
-        <v>102.22</v>
+        <v>4.44</v>
       </c>
       <c r="S10" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T10" s="9" t="inlineStr">
         <is>
@@ -21200,12 +21200,12 @@
       </c>
       <c r="U10" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.88€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V10" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 27/05/2025</t>
         </is>
       </c>
       <c r="W10" s="4" t="inlineStr">
@@ -21217,24 +21217,24 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>3402050002</t>
+          <t>3501100015</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>BRILLO PLANTA NATURAL 800ML</t>
+          <t>YNJECT CONECTOR PINO (NO VENTA)</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr"/>
       <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>ABONO NATURAL</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
@@ -21253,7 +21253,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="M11" s="5" t="n">
         <v>0</v>
@@ -21262,7 +21262,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P11" s="4" t="n">
         <v>92</v>
@@ -21283,7 +21283,7 @@
       </c>
       <c r="U11" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 45.88€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 5.88€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V11" s="4" t="inlineStr">
@@ -21300,24 +21300,24 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>3302210022</t>
+          <t>3501100026</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>COMPO FERTILIZANTE CICLAMENES 250ML</t>
+          <t>BIOFLOWER INSECTICIDA NATURAL NEEMEX 500ML</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr"/>
       <c r="D12" s="3" t="inlineStr"/>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>ABONOS</t>
+          <t>FITOSANITARIOS</t>
         </is>
       </c>
       <c r="G12" s="4" t="n">
@@ -21351,13 +21351,13 @@
         <v>92</v>
       </c>
       <c r="Q12" s="4" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="R12" s="4" t="n">
-        <v>102.22</v>
+        <v>17.78</v>
       </c>
       <c r="S12" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T12" s="9" t="inlineStr">
         <is>
@@ -21366,12 +21366,12 @@
       </c>
       <c r="U12" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 16.38€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V12" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 15/05/2025</t>
         </is>
       </c>
       <c r="W12" s="4" t="inlineStr">
@@ -21383,24 +21383,24 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>3501100022</t>
+          <t>3701010006</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>YNJECT GO PALMERAS (NO VENTA)</t>
+          <t>HERBICIDA DUO (FLUROXI + QUIZALOF)</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr"/>
       <c r="D13" s="3" t="inlineStr"/>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>HERBICIDAS</t>
         </is>
       </c>
       <c r="G13" s="4" t="n">
@@ -21419,7 +21419,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="M13" s="5" t="n">
         <v>0</v>
@@ -21428,7 +21428,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="P13" s="4" t="n">
         <v>92</v>
@@ -21449,7 +21449,7 @@
       </c>
       <c r="U13" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 211.68€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 71.75€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V13" s="4" t="inlineStr">
@@ -21466,24 +21466,24 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>3501100026</t>
+          <t>3402050002</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>BIOFLOWER INSECTICIDA NATURAL NEEMEX 500ML</t>
+          <t>BRILLO PLANTA NATURAL 800ML</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr"/>
       <c r="D14" s="3" t="inlineStr"/>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONO NATURAL</t>
         </is>
       </c>
       <c r="G14" s="4" t="n">
@@ -21502,7 +21502,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M14" s="5" t="n">
         <v>0</v>
@@ -21511,19 +21511,19 @@
         <v>0</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P14" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q14" s="4" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="R14" s="4" t="n">
-        <v>17.78</v>
+        <v>102.22</v>
       </c>
       <c r="S14" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T14" s="9" t="inlineStr">
         <is>
@@ -21532,12 +21532,12 @@
       </c>
       <c r="U14" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 45.88€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V14" s="4" t="inlineStr">
         <is>
-          <t>Compra 15/05/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W14" s="4" t="inlineStr">
@@ -21549,24 +21549,24 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>3501100021</t>
+          <t>3302210005</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>YNJECT GO PINO (NO VENTA)</t>
+          <t>CANABIUM VITACANN BIOESTIMULADOR 250ML</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr"/>
       <c r="D15" s="3" t="inlineStr"/>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>FITOSANITARIOS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G15" s="4" t="n">
@@ -21585,7 +21585,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="M15" s="5" t="n">
         <v>0</v>
@@ -21594,19 +21594,19 @@
         <v>0</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q15" s="4" t="n">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="R15" s="4" t="n">
-        <v>102.22</v>
+        <v>36.67</v>
       </c>
       <c r="S15" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T15" s="9" t="inlineStr">
         <is>
@@ -21615,12 +21615,12 @@
       </c>
       <c r="U15" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 47.04€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V15" s="4" t="inlineStr">
         <is>
-          <t>Stock inicial</t>
+          <t>Compra 28/04/2025</t>
         </is>
       </c>
       <c r="W15" s="4" t="inlineStr">
@@ -21632,12 +21632,12 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>3302210016</t>
+          <t>3301080002</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>VIGORIZANTE FOLIAR CACTUS Y CRASAS 250ML</t>
+          <t>COMPO REVIT ORQUIDEA MONODOSIS 5X30ML</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr"/>
@@ -21668,7 +21668,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="M16" s="5" t="n">
         <v>0</v>
@@ -21677,16 +21677,16 @@
         <v>0</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P16" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q16" s="4" t="n">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="R16" s="4" t="n">
-        <v>63.33</v>
+        <v>4.44</v>
       </c>
       <c r="S16" s="5" t="n">
         <v>0</v>
@@ -21703,7 +21703,7 @@
       </c>
       <c r="V16" s="4" t="inlineStr">
         <is>
-          <t>Compra 04/04/2025</t>
+          <t>Compra 27/05/2025</t>
         </is>
       </c>
       <c r="W16" s="4" t="inlineStr">
@@ -21715,24 +21715,24 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>3901160000</t>
+          <t>3302210022</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>FIN DESINFECTANTE SUPERFICIES 1L LU</t>
+          <t>COMPO FERTILIZANTE CICLAMENES 250ML</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr"/>
       <c r="D17" s="3" t="inlineStr"/>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>ANTI-PLAGAS</t>
+          <t>ABONOS</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
@@ -21766,13 +21766,13 @@
         <v>92</v>
       </c>
       <c r="Q17" s="4" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="R17" s="4" t="n">
-        <v>17.78</v>
+        <v>102.22</v>
       </c>
       <c r="S17" s="5" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T17" s="9" t="inlineStr">
         <is>
@@ -21781,12 +21781,12 @@
       </c>
       <c r="U17" s="3" t="inlineStr">
         <is>
-          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 0% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 0.0€. Prioridad máxima.</t>
+          <t>LIQUIDACIÓN URGENTE: Aplicar descuento 20% inmediato. Eliminar del catálogo próxima temporada. Capital liberado: 16.38€. Prioridad máxima.</t>
         </is>
       </c>
       <c r="V17" s="4" t="inlineStr">
         <is>
-          <t>Compra 15/05/2025</t>
+          <t>Stock inicial</t>
         </is>
       </c>
       <c r="W17" s="4" t="inlineStr">
@@ -21798,12 +21798,12 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>3502020004</t>
+          <t>3501010004</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>COMPO BIO FUNGICIDA STOP 750ML</t>
+          <t>TRIPLE ACCION 1000ML AFIDOR</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr"/>
@@ -21834,7 +21834,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>0</v>
@@ -21843,16 +21843,16 @@
         <v>0</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="P18" s="4" t="n">
         <v>92</v>
       </c>
       <c r="Q18" s="4" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="R18" s="4" t="n">
-        <v>4.44</v>
+        <v>36.67</v>
       </c>
       <c r="S18" s="5" t="n">
         <v>0</v>
@@ -21869,7 +21869,7 @@
       </c>
       <c r="V18" s="4" t="inlineStr">
         <is>
-          <t>Compra 27/05/2025</t>
+          <t>Compra 28/04/2025</t>
         </is>
       </c>
       <c r="W18" s="4" t="inlineStr">

</xml_diff>